<commit_message>
build: :construction: Se va agregando las funciones para el envio de correo atra vez de ZapSign
</commit_message>
<xml_diff>
--- a/public/contratos/Excel prueba de contrato.xlsx
+++ b/public/contratos/Excel prueba de contrato.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MaríaFernandaPradaCr\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QM\Desktop\contratos1\public\contratos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA28C9F4-352B-4642-8241-2CB559D6F582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B0A3D43-524F-45C1-9111-DC9F288C5F85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{154874EA-5800-4E6F-B81B-B598FC728375}"/>
   </bookViews>
@@ -3268,8 +3268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{658075FD-451C-4A05-8045-1F7769A17105}">
   <dimension ref="A1:V253"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3286,7 +3286,7 @@
     <col min="12" max="12" width="33.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3344,7 +3344,7 @@
       <c r="U1" s="4"/>
       <c r="V1" s="4"/>
     </row>
-    <row r="2" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="5"/>
       <c r="B2" s="6">
         <v>45875.555717592593</v>
@@ -3446,7 +3446,7 @@
       <c r="U3" s="11"/>
       <c r="V3" s="11"/>
     </row>
-    <row r="4" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="5"/>
       <c r="B4" s="6">
         <v>45875.603206018517</v>
@@ -3500,7 +3500,7 @@
       <c r="U4" s="11"/>
       <c r="V4" s="11"/>
     </row>
-    <row r="5" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="12"/>
       <c r="B5" s="6">
         <v>45875.626400462963</v>
@@ -3592,7 +3592,7 @@
       <c r="U6" s="11"/>
       <c r="V6" s="11"/>
     </row>
-    <row r="7" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="12"/>
       <c r="B7" s="6">
         <v>45875.636967592596</v>
@@ -3684,7 +3684,7 @@
       <c r="U8" s="11"/>
       <c r="V8" s="11"/>
     </row>
-    <row r="9" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="12"/>
       <c r="B9" s="6">
         <v>45877.459016203706</v>
@@ -3730,7 +3730,7 @@
       <c r="U9" s="11"/>
       <c r="V9" s="11"/>
     </row>
-    <row r="10" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="5"/>
       <c r="B10" s="6">
         <v>45877.469965277778</v>
@@ -3776,7 +3776,7 @@
       <c r="U10" s="11"/>
       <c r="V10" s="11"/>
     </row>
-    <row r="11" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="12"/>
       <c r="B11" s="6">
         <v>45877.472488425927</v>
@@ -3822,7 +3822,7 @@
       <c r="U11" s="11"/>
       <c r="V11" s="11"/>
     </row>
-    <row r="12" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="5"/>
       <c r="B12" s="6">
         <v>45877.488206018519</v>
@@ -3922,7 +3922,7 @@
       <c r="U13" s="11"/>
       <c r="V13" s="11"/>
     </row>
-    <row r="14" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="5"/>
       <c r="B14" s="6">
         <v>45878.374664351853</v>
@@ -3976,7 +3976,7 @@
       <c r="U14" s="11"/>
       <c r="V14" s="11"/>
     </row>
-    <row r="15" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="12"/>
       <c r="B15" s="6">
         <v>45878.375868055555</v>
@@ -4122,7 +4122,7 @@
       <c r="U17" s="11"/>
       <c r="V17" s="11"/>
     </row>
-    <row r="18" spans="1:22" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="5"/>
       <c r="B18" s="6">
         <v>45878.406574074077</v>
@@ -4214,7 +4214,7 @@
       <c r="U19" s="11"/>
       <c r="V19" s="11"/>
     </row>
-    <row r="20" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="5"/>
       <c r="B20" s="6">
         <v>45878.464918981481</v>
@@ -4260,7 +4260,7 @@
       <c r="U20" s="11"/>
       <c r="V20" s="11"/>
     </row>
-    <row r="21" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="23"/>
       <c r="B21" s="24">
         <v>45878.474409722221</v>
@@ -4360,7 +4360,7 @@
       <c r="U22" s="11"/>
       <c r="V22" s="11"/>
     </row>
-    <row r="23" spans="1:22" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="12"/>
       <c r="B23" s="6">
         <v>45878.489317129628</v>
@@ -4406,7 +4406,7 @@
       <c r="U23" s="11"/>
       <c r="V23" s="11"/>
     </row>
-    <row r="24" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="5"/>
       <c r="B24" s="6">
         <v>45878.503067129626</v>
@@ -4452,7 +4452,7 @@
       <c r="U24" s="11"/>
       <c r="V24" s="11"/>
     </row>
-    <row r="25" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="12"/>
       <c r="B25" s="6">
         <v>45879.828877314816</v>
@@ -4498,7 +4498,7 @@
       <c r="U25" s="11"/>
       <c r="V25" s="11"/>
     </row>
-    <row r="26" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="5"/>
       <c r="B26" s="6">
         <v>45879.896458333336</v>
@@ -4636,7 +4636,7 @@
       <c r="U28" s="11"/>
       <c r="V28" s="11"/>
     </row>
-    <row r="29" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="12"/>
       <c r="B29" s="6">
         <v>45880.525300925925</v>
@@ -4728,7 +4728,7 @@
       <c r="U30" s="11"/>
       <c r="V30" s="11"/>
     </row>
-    <row r="31" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="12"/>
       <c r="B31" s="6">
         <v>45880.536585648151</v>
@@ -4774,7 +4774,7 @@
       <c r="U31" s="11"/>
       <c r="V31" s="11"/>
     </row>
-    <row r="32" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="5"/>
       <c r="B32" s="6">
         <v>45880.539039351854</v>
@@ -5050,7 +5050,7 @@
       <c r="U37" s="11"/>
       <c r="V37" s="11"/>
     </row>
-    <row r="38" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="5"/>
       <c r="B38" s="6">
         <v>45880.797442129631</v>
@@ -5104,7 +5104,7 @@
       <c r="U38" s="11"/>
       <c r="V38" s="11"/>
     </row>
-    <row r="39" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="12"/>
       <c r="B39" s="6">
         <v>45881.493460648147</v>
@@ -5150,7 +5150,7 @@
       <c r="U39" s="11"/>
       <c r="V39" s="11"/>
     </row>
-    <row r="40" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="5"/>
       <c r="B40" s="6">
         <v>45881.509502314817</v>
@@ -5204,7 +5204,7 @@
       <c r="U40" s="11"/>
       <c r="V40" s="11"/>
     </row>
-    <row r="41" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="12"/>
       <c r="B41" s="6">
         <v>45881.621203703704</v>
@@ -5358,7 +5358,7 @@
       <c r="U43" s="11"/>
       <c r="V43" s="11"/>
     </row>
-    <row r="44" spans="1:22" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" s="5"/>
       <c r="B44" s="6">
         <v>45882.207835648151</v>
@@ -5412,7 +5412,7 @@
       <c r="U44" s="11"/>
       <c r="V44" s="11"/>
     </row>
-    <row r="45" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="12"/>
       <c r="B45" s="6">
         <v>45882.706354166665</v>
@@ -5550,7 +5550,7 @@
       <c r="U47" s="11"/>
       <c r="V47" s="11"/>
     </row>
-    <row r="48" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="5"/>
       <c r="B48" s="6">
         <v>45884.710613425923</v>
@@ -5650,7 +5650,7 @@
       <c r="U49" s="11"/>
       <c r="V49" s="11"/>
     </row>
-    <row r="50" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="5"/>
       <c r="B50" s="6">
         <v>45888.428136574075</v>
@@ -5696,7 +5696,7 @@
       <c r="U50" s="11"/>
       <c r="V50" s="11"/>
     </row>
-    <row r="51" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A51" s="12"/>
       <c r="B51" s="6">
         <v>45888.428761574076</v>
@@ -5742,7 +5742,7 @@
       <c r="U51" s="11"/>
       <c r="V51" s="11"/>
     </row>
-    <row r="52" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A52" s="30"/>
       <c r="B52" s="31">
         <v>45888.470763888887</v>
@@ -5788,7 +5788,7 @@
       <c r="U52" s="11"/>
       <c r="V52" s="11"/>
     </row>
-    <row r="53" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A53" s="12"/>
       <c r="B53" s="6">
         <v>45888.482407407406</v>
@@ -5834,7 +5834,7 @@
       <c r="U53" s="11"/>
       <c r="V53" s="11"/>
     </row>
-    <row r="54" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A54" s="5"/>
       <c r="B54" s="6">
         <v>45888.550613425927</v>
@@ -5880,7 +5880,7 @@
       <c r="U54" s="11"/>
       <c r="V54" s="11"/>
     </row>
-    <row r="55" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A55" s="34"/>
       <c r="B55" s="35">
         <v>45889.478055555555</v>
@@ -5972,7 +5972,7 @@
       <c r="U56" s="11"/>
       <c r="V56" s="11"/>
     </row>
-    <row r="57" spans="1:22" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A57" s="12"/>
       <c r="B57" s="6">
         <v>45891.716238425928</v>
@@ -6018,7 +6018,7 @@
       <c r="U57" s="11"/>
       <c r="V57" s="11"/>
     </row>
-    <row r="58" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A58" s="5"/>
       <c r="B58" s="6">
         <v>45895.757743055554</v>
@@ -6064,7 +6064,7 @@
       <c r="U58" s="11"/>
       <c r="V58" s="11"/>
     </row>
-    <row r="59" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A59" s="12"/>
       <c r="B59" s="6">
         <v>45895.761284722219</v>
@@ -6110,7 +6110,7 @@
       <c r="U59" s="11"/>
       <c r="V59" s="11"/>
     </row>
-    <row r="60" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A60" s="30"/>
       <c r="B60" s="36">
         <v>45896.566030092596</v>
@@ -6210,7 +6210,7 @@
       <c r="U61" s="11"/>
       <c r="V61" s="11"/>
     </row>
-    <row r="62" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A62" s="40"/>
       <c r="B62" s="41">
         <v>45898.71434027778</v>
@@ -6256,7 +6256,7 @@
       <c r="U62" s="11"/>
       <c r="V62" s="11"/>
     </row>
-    <row r="63" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A63" s="12"/>
       <c r="B63" s="6">
         <v>45904.006249999999</v>
@@ -6302,7 +6302,7 @@
       <c r="U63" s="11"/>
       <c r="V63" s="11"/>
     </row>
-    <row r="64" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A64" s="42" t="s">
         <v>301</v>
       </c>
@@ -6446,7 +6446,7 @@
       <c r="U66" s="11"/>
       <c r="V66" s="11"/>
     </row>
-    <row r="67" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A67" s="43" t="s">
         <v>301</v>
       </c>
@@ -6494,7 +6494,7 @@
       <c r="U67" s="11"/>
       <c r="V67" s="11"/>
     </row>
-    <row r="68" spans="1:22" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A68" s="42" t="s">
         <v>301</v>
       </c>
@@ -6590,7 +6590,7 @@
       <c r="U69" s="11"/>
       <c r="V69" s="11"/>
     </row>
-    <row r="70" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A70" s="42" t="s">
         <v>301</v>
       </c>
@@ -6638,7 +6638,7 @@
       <c r="U70" s="11"/>
       <c r="V70" s="11"/>
     </row>
-    <row r="71" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A71" s="43" t="s">
         <v>301</v>
       </c>
@@ -6742,7 +6742,7 @@
       <c r="U72" s="11"/>
       <c r="V72" s="11"/>
     </row>
-    <row r="73" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A73" s="43" t="s">
         <v>335</v>
       </c>
@@ -6790,7 +6790,7 @@
       <c r="U73" s="11"/>
       <c r="V73" s="11"/>
     </row>
-    <row r="74" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A74" s="42" t="s">
         <v>335</v>
       </c>
@@ -6894,7 +6894,7 @@
       <c r="U75" s="11"/>
       <c r="V75" s="11"/>
     </row>
-    <row r="76" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A76" s="42" t="s">
         <v>335</v>
       </c>
@@ -6950,7 +6950,7 @@
       <c r="U76" s="11"/>
       <c r="V76" s="11"/>
     </row>
-    <row r="77" spans="1:22" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A77" s="43" t="s">
         <v>335</v>
       </c>
@@ -6998,7 +6998,7 @@
       <c r="U77" s="11"/>
       <c r="V77" s="11"/>
     </row>
-    <row r="78" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A78" s="42" t="s">
         <v>335</v>
       </c>
@@ -7046,7 +7046,7 @@
       <c r="U78" s="11"/>
       <c r="V78" s="11"/>
     </row>
-    <row r="79" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A79" s="43" t="s">
         <v>335</v>
       </c>
@@ -7102,7 +7102,7 @@
       <c r="U79" s="11"/>
       <c r="V79" s="11"/>
     </row>
-    <row r="80" spans="1:22" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A80" s="42" t="s">
         <v>335</v>
       </c>
@@ -7150,7 +7150,7 @@
       <c r="U80" s="11"/>
       <c r="V80" s="11"/>
     </row>
-    <row r="81" spans="1:22" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A81" s="44" t="s">
         <v>335</v>
       </c>
@@ -7206,7 +7206,7 @@
       <c r="U81" s="11"/>
       <c r="V81" s="11"/>
     </row>
-    <row r="82" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A82" s="42" t="s">
         <v>335</v>
       </c>
@@ -7254,7 +7254,7 @@
       <c r="U82" s="11"/>
       <c r="V82" s="11"/>
     </row>
-    <row r="83" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A83" s="12"/>
       <c r="B83" s="6">
         <v>45993.637881944444</v>
@@ -7300,7 +7300,7 @@
       <c r="U83" s="11"/>
       <c r="V83" s="11"/>
     </row>
-    <row r="84" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A84" s="5"/>
       <c r="B84" s="6">
         <v>45993.638310185182</v>
@@ -7400,7 +7400,7 @@
       <c r="U85" s="11"/>
       <c r="V85" s="11"/>
     </row>
-    <row r="86" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A86" s="5"/>
       <c r="B86" s="6">
         <v>45993.681030092594</v>
@@ -7446,7 +7446,7 @@
       <c r="U86" s="11"/>
       <c r="V86" s="11"/>
     </row>
-    <row r="87" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A87" s="23"/>
       <c r="B87" s="24">
         <v>45994.368032407408</v>
@@ -7500,7 +7500,7 @@
       <c r="U87" s="11"/>
       <c r="V87" s="11"/>
     </row>
-    <row r="88" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A88" s="5"/>
       <c r="B88" s="6">
         <v>46002.732037037036</v>
@@ -7546,7 +7546,7 @@
       <c r="U88" s="11"/>
       <c r="V88" s="11"/>
     </row>
-    <row r="89" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A89" s="12"/>
       <c r="B89" s="6">
         <v>46006.580497685187</v>
@@ -7592,7 +7592,7 @@
       <c r="U89" s="11"/>
       <c r="V89" s="11"/>
     </row>
-    <row r="90" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A90" s="5"/>
       <c r="B90" s="6">
         <v>46006.730567129627</v>
@@ -7646,7 +7646,7 @@
       <c r="U90" s="11"/>
       <c r="V90" s="11"/>
     </row>
-    <row r="91" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A91" s="12"/>
       <c r="B91" s="6">
         <v>46006.730833333335</v>
@@ -7692,7 +7692,7 @@
       <c r="U91" s="11"/>
       <c r="V91" s="11"/>
     </row>
-    <row r="92" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A92" s="5"/>
       <c r="B92" s="6">
         <v>46006.732789351852</v>
@@ -7746,7 +7746,7 @@
       <c r="U92" s="11"/>
       <c r="V92" s="11"/>
     </row>
-    <row r="93" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A93" s="12"/>
       <c r="B93" s="45">
         <v>46006.732881944445</v>
@@ -7792,7 +7792,7 @@
       <c r="U93" s="11"/>
       <c r="V93" s="11"/>
     </row>
-    <row r="94" spans="1:22" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A94" s="46"/>
       <c r="B94" s="47">
         <v>46006.733865740738</v>
@@ -7846,7 +7846,7 @@
       <c r="U94" s="11"/>
       <c r="V94" s="11"/>
     </row>
-    <row r="95" spans="1:22" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A95" s="12"/>
       <c r="B95" s="45">
         <v>46006.750949074078</v>
@@ -7900,7 +7900,7 @@
       <c r="U95" s="11"/>
       <c r="V95" s="11"/>
     </row>
-    <row r="96" spans="1:22" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A96" s="46"/>
       <c r="B96" s="47">
         <v>46006.753113425926</v>
@@ -7946,7 +7946,7 @@
       <c r="U96" s="11"/>
       <c r="V96" s="11"/>
     </row>
-    <row r="97" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A97" s="12"/>
       <c r="B97" s="6">
         <v>46006.757071759261</v>
@@ -8000,7 +8000,7 @@
       <c r="U97" s="11"/>
       <c r="V97" s="11"/>
     </row>
-    <row r="98" spans="1:22" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A98" s="5"/>
       <c r="B98" s="6">
         <v>46006.762337962966</v>
@@ -8054,7 +8054,7 @@
       <c r="U98" s="11"/>
       <c r="V98" s="11"/>
     </row>
-    <row r="99" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A99" s="12"/>
       <c r="B99" s="6">
         <v>46006.769791666666</v>
@@ -8108,7 +8108,7 @@
       <c r="U99" s="11"/>
       <c r="V99" s="11"/>
     </row>
-    <row r="100" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A100" s="5"/>
       <c r="B100" s="6">
         <v>46006.77516203704</v>
@@ -8154,7 +8154,7 @@
       <c r="U100" s="11"/>
       <c r="V100" s="11"/>
     </row>
-    <row r="101" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A101" s="12"/>
       <c r="B101" s="6">
         <v>46006.781215277777</v>
@@ -8208,7 +8208,7 @@
       <c r="U101" s="11"/>
       <c r="V101" s="11"/>
     </row>
-    <row r="102" spans="1:22" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A102" s="5"/>
       <c r="B102" s="6">
         <v>46006.829513888886</v>
@@ -8254,7 +8254,7 @@
       <c r="U102" s="11"/>
       <c r="V102" s="11"/>
     </row>
-    <row r="103" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A103" s="12"/>
       <c r="B103" s="6">
         <v>46006.832638888889</v>
@@ -8300,7 +8300,7 @@
       <c r="U103" s="11"/>
       <c r="V103" s="11"/>
     </row>
-    <row r="104" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A104" s="5"/>
       <c r="B104" s="6">
         <v>46006.890879629631</v>
@@ -8346,7 +8346,7 @@
       <c r="U104" s="11"/>
       <c r="V104" s="11"/>
     </row>
-    <row r="105" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A105" s="12"/>
       <c r="B105" s="6">
         <v>46006.891736111109</v>
@@ -8392,7 +8392,7 @@
       <c r="U105" s="11"/>
       <c r="V105" s="11"/>
     </row>
-    <row r="106" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A106" s="5"/>
       <c r="B106" s="6">
         <v>46006.919062499997</v>
@@ -8438,7 +8438,7 @@
       <c r="U106" s="11"/>
       <c r="V106" s="11"/>
     </row>
-    <row r="107" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A107" s="12"/>
       <c r="B107" s="48">
         <v>46006.92559027778</v>
@@ -8492,7 +8492,7 @@
       <c r="U107" s="11"/>
       <c r="V107" s="11"/>
     </row>
-    <row r="108" spans="1:22" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A108" s="5"/>
       <c r="B108" s="6">
         <v>46006.944386574076</v>
@@ -8546,7 +8546,7 @@
       <c r="U108" s="11"/>
       <c r="V108" s="11"/>
     </row>
-    <row r="109" spans="1:22" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A109" s="12"/>
       <c r="B109" s="6">
         <v>46006.96166666667</v>
@@ -8600,7 +8600,7 @@
       <c r="U109" s="11"/>
       <c r="V109" s="11"/>
     </row>
-    <row r="110" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A110" s="5"/>
       <c r="B110" s="6">
         <v>46006.97378472222</v>
@@ -8646,7 +8646,7 @@
       <c r="U110" s="11"/>
       <c r="V110" s="11"/>
     </row>
-    <row r="111" spans="1:22" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A111" s="12"/>
       <c r="B111" s="6">
         <v>46007.1796412037</v>
@@ -8700,7 +8700,7 @@
       <c r="U111" s="11"/>
       <c r="V111" s="11"/>
     </row>
-    <row r="112" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A112" s="5"/>
       <c r="B112" s="6">
         <v>46007.206076388888</v>
@@ -8754,7 +8754,7 @@
       <c r="U112" s="11"/>
       <c r="V112" s="11"/>
     </row>
-    <row r="113" spans="1:22" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A113" s="12"/>
       <c r="B113" s="6">
         <v>46007.251354166663</v>
@@ -8808,7 +8808,7 @@
       <c r="U113" s="11"/>
       <c r="V113" s="11"/>
     </row>
-    <row r="114" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A114" s="5"/>
       <c r="B114" s="6">
         <v>46007.323703703703</v>
@@ -8862,7 +8862,7 @@
       <c r="U114" s="11"/>
       <c r="V114" s="11"/>
     </row>
-    <row r="115" spans="1:22" ht="78.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A115" s="12"/>
       <c r="B115" s="6">
         <v>46007.403368055559</v>
@@ -8916,7 +8916,7 @@
       <c r="U115" s="11"/>
       <c r="V115" s="11"/>
     </row>
-    <row r="116" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A116" s="5"/>
       <c r="B116" s="6">
         <v>46014.57371527778</v>
@@ -8970,7 +8970,7 @@
       <c r="U116" s="11"/>
       <c r="V116" s="11"/>
     </row>
-    <row r="117" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A117" s="12"/>
       <c r="B117" s="6">
         <v>46014.586192129631</v>
@@ -9024,7 +9024,7 @@
       <c r="U117" s="11"/>
       <c r="V117" s="11"/>
     </row>
-    <row r="118" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A118" s="5"/>
       <c r="B118" s="6">
         <v>46049.920532407406</v>
@@ -9078,7 +9078,7 @@
       <c r="U118" s="11"/>
       <c r="V118" s="11"/>
     </row>
-    <row r="119" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A119" s="12"/>
       <c r="B119" s="6">
         <v>46050.426030092596</v>
@@ -9132,7 +9132,7 @@
       <c r="U119" s="11"/>
       <c r="V119" s="11"/>
     </row>
-    <row r="120" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A120" s="5"/>
       <c r="B120" s="6">
         <v>46050.494062500002</v>
@@ -9178,7 +9178,7 @@
       <c r="U120" s="11"/>
       <c r="V120" s="11"/>
     </row>
-    <row r="121" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="121" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A121" s="12"/>
       <c r="B121" s="6">
         <v>46050.546689814815</v>
@@ -9224,7 +9224,7 @@
       <c r="U121" s="11"/>
       <c r="V121" s="11"/>
     </row>
-    <row r="122" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="122" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A122" s="5"/>
       <c r="B122" s="6">
         <v>46050.606516203705</v>
@@ -9278,7 +9278,7 @@
       <c r="U122" s="11"/>
       <c r="V122" s="11"/>
     </row>
-    <row r="123" spans="1:22" ht="65.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="123" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A123" s="12"/>
       <c r="B123" s="6">
         <v>46050.763807870368</v>
@@ -9324,7 +9324,7 @@
       <c r="U123" s="11"/>
       <c r="V123" s="11"/>
     </row>
-    <row r="124" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="124" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A124" s="5"/>
       <c r="B124" s="6">
         <v>46051.481249999997</v>
@@ -9370,7 +9370,7 @@
       <c r="U124" s="11"/>
       <c r="V124" s="11"/>
     </row>
-    <row r="125" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="125" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A125" s="12"/>
       <c r="B125" s="6">
         <v>46051.651400462964</v>
@@ -9416,7 +9416,7 @@
       <c r="U125" s="11"/>
       <c r="V125" s="11"/>
     </row>
-    <row r="126" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="126" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A126" s="5"/>
       <c r="B126" s="6">
         <v>46056.336643518516</v>
@@ -9462,7 +9462,7 @@
       <c r="U126" s="11"/>
       <c r="V126" s="11"/>
     </row>
-    <row r="127" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="127" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A127" s="12"/>
       <c r="B127" s="6">
         <v>46058.329814814817</v>
@@ -9516,7 +9516,7 @@
       <c r="U127" s="11"/>
       <c r="V127" s="11"/>
     </row>
-    <row r="128" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="128" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A128" s="5"/>
       <c r="B128" s="6">
         <v>46058.331157407411</v>
@@ -9570,7 +9570,7 @@
       <c r="U128" s="11"/>
       <c r="V128" s="11"/>
     </row>
-    <row r="129" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="129" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A129" s="12"/>
       <c r="B129" s="6">
         <v>46058.333460648151</v>
@@ -9616,7 +9616,7 @@
       <c r="U129" s="11"/>
       <c r="V129" s="11"/>
     </row>
-    <row r="130" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="130" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A130" s="5"/>
       <c r="B130" s="6">
         <v>46058.342129629629</v>
@@ -9662,7 +9662,7 @@
       <c r="U130" s="11"/>
       <c r="V130" s="11"/>
     </row>
-    <row r="131" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="131" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A131" s="12"/>
       <c r="B131" s="6">
         <v>46058.364699074074</v>
@@ -9708,7 +9708,7 @@
       <c r="U131" s="11"/>
       <c r="V131" s="11"/>
     </row>
-    <row r="132" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="132" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A132" s="5"/>
       <c r="B132" s="6">
         <v>46058.38853009259</v>
@@ -9762,7 +9762,7 @@
       <c r="U132" s="11"/>
       <c r="V132" s="11"/>
     </row>
-    <row r="133" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="133" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A133" s="12"/>
       <c r="B133" s="6">
         <v>46058.393854166665</v>
@@ -9816,7 +9816,7 @@
       <c r="U133" s="11"/>
       <c r="V133" s="11"/>
     </row>
-    <row r="134" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="134" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A134" s="5"/>
       <c r="B134" s="6">
         <v>46058.403356481482</v>
@@ -9870,7 +9870,7 @@
       <c r="U134" s="11"/>
       <c r="V134" s="11"/>
     </row>
-    <row r="135" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="135" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A135" s="12"/>
       <c r="B135" s="6">
         <v>46058.440949074073</v>
@@ -9916,7 +9916,7 @@
       <c r="U135" s="11"/>
       <c r="V135" s="11"/>
     </row>
-    <row r="136" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="136" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A136" s="5"/>
       <c r="B136" s="6">
         <v>46058.443368055552</v>
@@ -9970,7 +9970,7 @@
       <c r="U136" s="11"/>
       <c r="V136" s="11"/>
     </row>
-    <row r="137" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="137" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A137" s="12"/>
       <c r="B137" s="6">
         <v>46058.454375000001</v>
@@ -10016,7 +10016,7 @@
       <c r="U137" s="11"/>
       <c r="V137" s="11"/>
     </row>
-    <row r="138" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="138" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A138" s="5"/>
       <c r="B138" s="6">
         <v>46058.457152777781</v>
@@ -10062,7 +10062,7 @@
       <c r="U138" s="11"/>
       <c r="V138" s="11"/>
     </row>
-    <row r="139" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="139" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A139" s="12"/>
       <c r="B139" s="6">
         <v>46058.589421296296</v>
@@ -10108,7 +10108,7 @@
       <c r="U139" s="11"/>
       <c r="V139" s="11"/>
     </row>
-    <row r="140" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="140" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A140" s="5"/>
       <c r="B140" s="6">
         <v>46058.591319444444</v>
@@ -10270,7 +10270,7 @@
       <c r="U142" s="11"/>
       <c r="V142" s="11"/>
     </row>
-    <row r="143" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="143" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A143" s="12"/>
       <c r="B143" s="6">
         <v>46058.802395833336</v>
@@ -10324,7 +10324,7 @@
       <c r="U143" s="11"/>
       <c r="V143" s="11"/>
     </row>
-    <row r="144" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="144" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A144" s="5"/>
       <c r="B144" s="6">
         <v>46058.836041666669</v>
@@ -10378,7 +10378,7 @@
       <c r="U144" s="11"/>
       <c r="V144" s="11"/>
     </row>
-    <row r="145" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="145" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A145" s="34"/>
       <c r="B145" s="35">
         <v>46058.863032407404</v>
@@ -10432,7 +10432,7 @@
       <c r="U145" s="11"/>
       <c r="V145" s="11"/>
     </row>
-    <row r="146" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="146" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A146" s="5"/>
       <c r="B146" s="6">
         <v>46058.898275462961</v>
@@ -10486,7 +10486,7 @@
       <c r="U146" s="11"/>
       <c r="V146" s="11"/>
     </row>
-    <row r="147" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="147" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A147" s="12"/>
       <c r="B147" s="6">
         <v>46058.914259259262</v>
@@ -10586,7 +10586,7 @@
       <c r="U148" s="11"/>
       <c r="V148" s="11"/>
     </row>
-    <row r="149" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="149" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A149" s="12"/>
       <c r="B149" s="6">
         <v>46059.478587962964</v>
@@ -10640,7 +10640,7 @@
       <c r="U149" s="11"/>
       <c r="V149" s="11"/>
     </row>
-    <row r="150" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="150" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A150" s="5"/>
       <c r="B150" s="6">
         <v>46059.633344907408</v>
@@ -10740,7 +10740,7 @@
       <c r="U151" s="11"/>
       <c r="V151" s="11"/>
     </row>
-    <row r="152" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="152" spans="1:22" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A152" s="5"/>
       <c r="B152" s="6">
         <v>46062.374236111114</v>
@@ -10794,7 +10794,7 @@
       <c r="U152" s="11"/>
       <c r="V152" s="11"/>
     </row>
-    <row r="153" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="153" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A153" s="34"/>
       <c r="B153" s="35">
         <v>46062.418194444443</v>
@@ -10840,7 +10840,7 @@
       <c r="U153" s="11"/>
       <c r="V153" s="11"/>
     </row>
-    <row r="154" spans="1:22" ht="52.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="154" spans="1:22" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A154" s="49"/>
       <c r="B154" s="50">
         <v>46062.669456018521</v>
@@ -13264,5 +13264,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>